<commit_message>
Practicing the push and pull
</commit_message>
<xml_diff>
--- a/Data Files/Data.xlsx
+++ b/Data Files/Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,10 @@
     <t>Appointment Date</t>
   </si>
   <si>
-    <t>John Test111</t>
-  </si>
-  <si>
     <t>Vtest@123</t>
+  </si>
+  <si>
+    <t>John Test1112</t>
   </si>
 </sst>
 </file>
@@ -108,6 +108,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -155,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,7 +193,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,19 +405,19 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -448,12 +451,12 @@
         <v>44684</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +473,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -482,7 +485,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>